<commit_message>
Update with more user data
</commit_message>
<xml_diff>
--- a/Evaluation study results/FS-Evaluation-Survey-Responses.xlsx
+++ b/Evaluation study results/FS-Evaluation-Survey-Responses.xlsx
@@ -1,42 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10916"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10119"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jingwu/Documents/GitHub/DietCoach_appendix/Evaluation study results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13E4C35D-9516-C84F-B3D6-00F6C898B572}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A3DD41E-F14C-AD44-AC20-8B5127ED8AD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="-700" windowWidth="38400" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="608" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1538" uniqueCount="183">
   <si>
     <t>ID</t>
   </si>
@@ -302,9 +291,6 @@
     <t>Fände es wichtig, dass bei Mehrpersonenhaushalte die demografische Daten des gesamten Haushalts erfasst wird. So lassen sich die Einkäufe besser interpretieren.</t>
   </si>
   <si>
-    <t>Für konkrete Fragen bzgl. Lebensmitteln z.B. FODMAP Gehalt</t>
-  </si>
-  <si>
     <t>30</t>
   </si>
   <si>
@@ -329,12 +315,6 @@
     <t>0</t>
   </si>
   <si>
-    <t>in Abhängigkeit des Bedürnfis / Interesses und Bedarfs meiner Patient:innen</t>
-  </si>
-  <si>
-    <t>das kann ich noch nicht sagen</t>
-  </si>
-  <si>
     <t xml:space="preserve">Wir unterscheiden NICHT in "gute" und "schlechte" Lebensmittel! / sagt nichts über die tatsächliche Einnahme aus z.B. wenn jemand 1kg Reis kauft, bedeutet dies nicht, dass die Person das ganze kilo isst = erleichtert unsere Arbeit nicht, wir müssen trotzdem eine Ernährungsanamnese machen / denke für Makronährstoffaufnahme nicht sinnvoll. ev. eher zur Beurteilung von Mikronährstoffen z.B. ob und welche calciumreichen Lebensmittel eingekauft werden / Datenschutz? / denke wenn Pat. dies wissen, dass wir diese Daten sehen, gehen sie einfach ohne Cumulus einkaufen = Zweck verfehlt / wir machen schon jetzt genaue Produktempfehlungen in den Beratungen, der Online Shop ist dazu völlig ausreichend und ermöglicht uns auch zwischen verschiedenen Anbietern zu vergleichen und nicht nur die Produkte von Mirgso, Coop zu berücksichtigen </t>
   </si>
   <si>
@@ -363,6 +343,237 @@
   </si>
   <si>
     <t>Im stationären Setting würde ich die App eher nicht nutzen</t>
+  </si>
+  <si>
+    <t>42</t>
+  </si>
+  <si>
+    <t>Männlich</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>Allergien</t>
+  </si>
+  <si>
+    <t>Auswertung / Analyse der Einkaufsgewohnheiten</t>
+  </si>
+  <si>
+    <t>für Allergien und Unverträglichkeiten Screening, mögliche Diätfehler erkennen</t>
+  </si>
+  <si>
+    <t>33</t>
+  </si>
+  <si>
+    <t>Einkaufszettel ist seehr persönlich (wird wahrsch. auch als seehr persönlich wahrgenommen); Bereitschaft zur Transparenz???</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>punktuell, nicht dauerhaft (z.B. während 2-4 Sitzungen) nebst anderen Themen/Instrumenten.</t>
+  </si>
+  <si>
+    <t>Profil finde ich nicht nötig (persönliche Daten wie BMI).</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>48</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>41-60%</t>
+  </si>
+  <si>
+    <t>200</t>
+  </si>
+  <si>
+    <t>waere nur im ambulanten Bereich moeglich und nicht bei mehrfamilienhaushalten</t>
+  </si>
+  <si>
+    <t>keine Ahnung</t>
+  </si>
+  <si>
+    <t>ich berate gerne persoenlich, die app wuerde dazu fuehren, dass ich mehr am Bildschirm sitzen wuerde</t>
+  </si>
+  <si>
+    <t>34</t>
+  </si>
+  <si>
+    <t>Patienten können weniger gut miteinbezogen werden für eine Intervention. Es gibt immer mehrere Möglichkeiten ein Ziel (z.B. Gewichtsziel) zu erreichen.</t>
+  </si>
+  <si>
+    <t>Allenfalls während der Beratung die Einkäufe zusammen mit den Patienten anschauen und anhand eines Beratungsgesprächs Interventionen treffen</t>
+  </si>
+  <si>
+    <t>Weitere Schwierigkeit: bei Vorrateinkäufen kann nicht auf eine einzelnen Tag oder Woche geschlossen werden</t>
+  </si>
+  <si>
+    <t>29</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wenn die Person garnicht viel selbst kocht sondern in einer Kantine, Auswärts isst oder Geschäftlich viel unterwegs ist und dann auf dem Weg isst. </t>
+  </si>
+  <si>
+    <t>Ab und Zu max in 2-3 Beratungen, weil es zwar Informationen liefert aber nicht sehr verhaltenstherapeutisch ist.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Es zielt auf die Informationsgewinnung und nicht auf die Verhaltensveränderung, was ist der Grund das die Person so einkauft, diese Infos fehlen. </t>
+  </si>
+  <si>
+    <t>43</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>zur Analyse er regelmässigen Einkäufe</t>
+  </si>
+  <si>
+    <t>Vermutlich nur bei Adipositas, Diabetes und Dyslipidämie Patient*innen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Die Suchfunktion müsste schneller sein, man sollte nicht ewig scrollen müssen. </t>
+  </si>
+  <si>
+    <t>35</t>
+  </si>
+  <si>
+    <t>500</t>
+  </si>
+  <si>
+    <t>in ambulanten Beratungen</t>
+  </si>
+  <si>
+    <t>unklar wie viel wirklich gegessen wurde. Es gibt guten Überblick auf die Produkteauswahl.</t>
+  </si>
+  <si>
+    <t>32</t>
+  </si>
+  <si>
+    <t>100</t>
+  </si>
+  <si>
+    <t>In anbulanten Beratungen</t>
+  </si>
+  <si>
+    <t>besser gefilterte Suchfunktion</t>
+  </si>
+  <si>
+    <t>150</t>
+  </si>
+  <si>
+    <t>Ambulanten Setting</t>
+  </si>
+  <si>
+    <t>Eine Chatfunktion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ich denke die Limitation sind noch sehr gross. </t>
+  </si>
+  <si>
+    <t>bei Adipositas ggf. als Art Onlineberatung (wenn Pat 100 % bei Migros / Coop einkaufen)</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>Interpretation der Einkäufe der Patienten, Einblick zur Lebensmittelauswahl gewinnen</t>
+  </si>
+  <si>
+    <t>Interaktiver, Notizen der Pat., FAQ, Vergleich zur Lebemsmittelpyramide, Möglichkeit zur Erstellung Ernährungsprotokolls und Vergleich mit Lebensmittelpyramide.</t>
+  </si>
+  <si>
+    <t>tolle Arbeit</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>Stimme überhaupt nicht  zu</t>
+  </si>
+  <si>
+    <t>neben der Empfehlung vielleicht auch eine Feedbackfunktion bei Fortschritt was gut umgesetzt wurde</t>
+  </si>
+  <si>
+    <t>in einer digitalen Beratung</t>
+  </si>
+  <si>
+    <t>Chatfunktion</t>
+  </si>
+  <si>
+    <t>Produkte die man auswählen kann sehr speziell, lange Suche, dann wird man das System nicht nutzen</t>
+  </si>
+  <si>
+    <t>Einkommensklasse</t>
+  </si>
+  <si>
+    <t>Bei Adipositas Patienten, Stoffwechselerkrankten, DM...</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chat Funktion, </t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>0.5</t>
+  </si>
+  <si>
+    <t>Einkaufsgewohnheiten ansehen</t>
+  </si>
+  <si>
+    <t>Pat. sollten rein schreiben können, ob dies eher ein gewöhnlicher Einkauf war oder für spezielle Anlässe.</t>
+  </si>
+  <si>
+    <t>Portionsgrösse und wie viel wurde in welche Zeutrahmen gegessen.</t>
+  </si>
+  <si>
+    <t>Im Moment würde ich es nicht nutzen.</t>
+  </si>
+  <si>
+    <t>Berücksichtigung von Portionsgrößen, tatsächlich verzehrten Mengen und Verzehrszeiträumen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zum Erfassen der Ernährungsgewohnheiten der Patienten/innen </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nicht klar ersichtlich, was in einem Mehrpersonen Haushalt von wem konsumiert wird. </t>
+  </si>
+  <si>
+    <t>Ich sehe den Mehrwert noch nicht so ganz. Negativ: Häufigkeit der Einkaufe und Verteilung auf die Tage. Aufteilung auf die Personen im Haushalt. Das Teilen von Einkaufsdaten an Krankenkassen sehe ich kritisch.</t>
+  </si>
+  <si>
+    <t>Energiebedarf einer Person, Aussertorts-Essen (Take away)</t>
+  </si>
+  <si>
+    <t>90</t>
+  </si>
+  <si>
+    <t>Ja, u. U., dass sie kompakter wird, für viele ERB's wäre eine solche App viel zu aufwendig (für ERB's im Alltag ein enorm grosser Datensatz, welche hier dargestellt wird und nicht so auf die schnelle einen Überblick gibt).</t>
+  </si>
+  <si>
+    <t>kompaktere Übersicht (z.B. Nutriscore ist meist im klinischen Alltag für ERB weniger von Interesse, Nährstoffe reichen aus), es braucht zudem unbedingt eine Energiebedarfsformel, damit die En% von Makronährstoffen in Relation stehen (Energiebedarfsformel könnte daher gut in die App integriert werden in den Profil-Stammdaten)</t>
+  </si>
+  <si>
+    <t>Allgemeine Datenschutz-technische Bedenken, weiters: Tracking von Kaufverhalten von Patient*innen kann auch Druck bei Pat. auslösen (wenn Pat. weiss, das ERB diese Daten direkt einsehen kann)</t>
+  </si>
+  <si>
+    <t>Food waste Daten, die Möglichkeit einzelne Zutaten in die Auswertung zu integrieren, es wäre nützlich direkt zu wissen ob es ein "spezieller" Einkauf war</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eher um einen groben Überblich in die Einkaufsgewohnheiten der Patienten zu erhalten </t>
+  </si>
+  <si>
+    <t>Es sind noch sehr viele Fragen, welche ich den Patienten stellen müsste, daher würde sich meine Arbeit möglicherweise nicht verschnellern. Daher würde ich Überprüfungsmöglichkeiten integrieren, das sdie Pazienten z.B im Voraus angeben müssten, ob es spezielle Einküfe waren, für welchen Zeitraum sie eingekauft haben, wie viel sie von dem Einkauf verzehrt haben usw. Auch möglicherweise einzelne Zutaten integrieren und falls möglich berechnungen über Food Waste</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ich war am Anfang nicht sehr sicher in der Nutzung (wie was finden und bewerten). Glaube aber, das mann das schnell gut im Griff haben kann. Leider kann ich gewisse Fragen nicht konkret beantworten, da ich urzeit keine Patienten berate. </t>
   </si>
 </sst>
 </file>
@@ -370,7 +581,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="m/d/yy\ h:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="m/d/yy\ h:mm:ss"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -403,7 +614,7 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -555,10 +766,10 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="m/d/yy\ h:mm:ss"/>
+      <numFmt numFmtId="165" formatCode="m/d/yy\ h:mm:ss"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="m/d/yy\ h:mm:ss"/>
+      <numFmt numFmtId="165" formatCode="m/d/yy\ h:mm:ss"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -577,8 +788,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:AY13" totalsRowShown="0">
-  <autoFilter ref="A1:AY13" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:AY33" totalsRowShown="0">
+  <autoFilter ref="A1:AY33" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="51">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ID" dataDxfId="50"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Start time" dataDxfId="49"/>
@@ -933,10 +1144,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AY13"/>
+  <dimension ref="A1:AY33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AG1" workbookViewId="0">
-      <selection activeCell="AW4" sqref="AW4"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2001,79 +2212,79 @@
     </row>
     <row r="8" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B8" s="1">
-        <v>45540.5317476852</v>
+        <v>45540.533576388902</v>
       </c>
       <c r="C8" s="1">
-        <v>45540.542175925897</v>
+        <v>45540.542326388902</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>72</v>
+        <v>88</v>
       </c>
       <c r="E8" t="s">
         <v>52</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>84</v>
+        <v>53</v>
       </c>
       <c r="G8" t="s">
         <v>54</v>
       </c>
       <c r="H8" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="I8" t="s">
+        <v>79</v>
+      </c>
+      <c r="J8" t="s">
+        <v>79</v>
+      </c>
+      <c r="K8" t="s">
+        <v>54</v>
+      </c>
+      <c r="L8" t="s">
+        <v>55</v>
+      </c>
+      <c r="M8" t="s">
+        <v>55</v>
+      </c>
+      <c r="N8" t="s">
+        <v>58</v>
+      </c>
+      <c r="O8" t="s">
         <v>57</v>
       </c>
-      <c r="J8" t="s">
-        <v>57</v>
-      </c>
-      <c r="K8" t="s">
-        <v>54</v>
-      </c>
-      <c r="L8" t="s">
-        <v>55</v>
-      </c>
-      <c r="M8" t="s">
-        <v>54</v>
-      </c>
-      <c r="N8" t="s">
-        <v>55</v>
-      </c>
-      <c r="O8" t="s">
-        <v>55</v>
-      </c>
       <c r="P8" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="Q8" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="R8" t="s">
-        <v>57</v>
+        <v>79</v>
       </c>
       <c r="S8" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="T8" t="s">
-        <v>57</v>
+        <v>79</v>
       </c>
       <c r="U8" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="V8" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="W8" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="X8" t="s">
-        <v>58</v>
+        <v>79</v>
       </c>
       <c r="Y8" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="Z8" t="s">
         <v>54</v>
@@ -2082,7 +2293,7 @@
         <v>58</v>
       </c>
       <c r="AB8" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="AC8" t="s">
         <v>58</v>
@@ -2091,19 +2302,19 @@
         <v>54</v>
       </c>
       <c r="AE8" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="AF8" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="AG8" t="s">
         <v>58</v>
       </c>
       <c r="AH8" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="AI8" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="AJ8" t="s">
         <v>58</v>
@@ -2129,40 +2340,49 @@
       <c r="AQ8" t="s">
         <v>58</v>
       </c>
+      <c r="AR8" t="s">
+        <v>89</v>
+      </c>
       <c r="AS8" t="s">
-        <v>58</v>
+        <v>79</v>
       </c>
       <c r="AT8" t="s">
-        <v>56</v>
+        <v>79</v>
       </c>
       <c r="AU8" t="s">
-        <v>58</v>
+        <v>79</v>
       </c>
       <c r="AV8" s="2" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="AW8" t="s">
-        <v>88</v>
+        <v>90</v>
+      </c>
+      <c r="AX8" t="s">
+        <v>91</v>
+      </c>
+      <c r="AY8" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="9" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B9" s="1">
-        <v>45540.533576388902</v>
+        <v>45540.5335416667</v>
       </c>
       <c r="C9" s="1">
-        <v>45540.542326388902</v>
+        <v>45540.542615740698</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="E9" t="s">
         <v>52</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>53</v>
+        <v>73</v>
       </c>
       <c r="G9" t="s">
         <v>54</v>
@@ -2174,85 +2394,85 @@
         <v>79</v>
       </c>
       <c r="J9" t="s">
-        <v>79</v>
+        <v>57</v>
       </c>
       <c r="K9" t="s">
         <v>54</v>
       </c>
       <c r="L9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="M9" t="s">
         <v>55</v>
       </c>
       <c r="N9" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="O9" t="s">
+        <v>54</v>
+      </c>
+      <c r="P9" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q9" t="s">
         <v>57</v>
-      </c>
-      <c r="P9" t="s">
-        <v>56</v>
-      </c>
-      <c r="Q9" t="s">
-        <v>58</v>
       </c>
       <c r="R9" t="s">
         <v>79</v>
       </c>
       <c r="S9" t="s">
-        <v>58</v>
+        <v>79</v>
       </c>
       <c r="T9" t="s">
         <v>79</v>
       </c>
       <c r="U9" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="V9" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="W9" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="X9" t="s">
         <v>79</v>
       </c>
       <c r="Y9" t="s">
-        <v>56</v>
+        <v>79</v>
       </c>
       <c r="Z9" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="AA9" t="s">
-        <v>58</v>
+        <v>79</v>
       </c>
       <c r="AB9" t="s">
         <v>56</v>
       </c>
       <c r="AC9" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="AD9" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="AE9" t="s">
-        <v>54</v>
+        <v>79</v>
       </c>
       <c r="AF9" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="AG9" t="s">
-        <v>58</v>
+        <v>79</v>
       </c>
       <c r="AH9" t="s">
         <v>58</v>
       </c>
       <c r="AI9" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="AJ9" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="AK9" t="s">
         <v>74</v>
@@ -2264,19 +2484,19 @@
         <v>60</v>
       </c>
       <c r="AN9" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="AO9" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="AP9" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="AQ9" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="AR9" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="AS9" t="s">
         <v>79</v>
@@ -2288,48 +2508,48 @@
         <v>79</v>
       </c>
       <c r="AV9" s="2" t="s">
-        <v>84</v>
+        <v>68</v>
       </c>
       <c r="AW9" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="AX9" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="AY9" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
     </row>
     <row r="10" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B10" s="1">
-        <v>45540.537685185198</v>
+        <v>45540.537314814799</v>
       </c>
       <c r="C10" s="1">
-        <v>45540.542488425897</v>
+        <v>45540.542638888903</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="E10" t="s">
         <v>52</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="G10" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="H10" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="I10" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="J10" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="K10" t="s">
         <v>55</v>
@@ -2341,82 +2561,82 @@
         <v>55</v>
       </c>
       <c r="N10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="O10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="P10" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="Q10" t="s">
         <v>56</v>
       </c>
       <c r="R10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="S10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="T10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="U10" t="s">
         <v>56</v>
       </c>
       <c r="V10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="W10" t="s">
         <v>56</v>
       </c>
       <c r="X10" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="Y10" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="Z10" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="AA10" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="AB10" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="AC10" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="AD10" t="s">
         <v>54</v>
       </c>
       <c r="AE10" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="AF10" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="AG10" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="AH10" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="AI10" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="AJ10" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="AK10" t="s">
         <v>74</v>
       </c>
       <c r="AL10" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="AM10" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="AN10" t="s">
         <v>54</v>
@@ -2425,42 +2645,36 @@
         <v>54</v>
       </c>
       <c r="AP10" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="AQ10" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="AS10" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="AT10" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="AU10" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="AV10" s="2" t="s">
-        <v>96</v>
+        <v>68</v>
       </c>
       <c r="AW10" t="s">
-        <v>97</v>
-      </c>
-      <c r="AX10" t="s">
-        <v>98</v>
-      </c>
-      <c r="AY10" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
     </row>
     <row r="11" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B11" s="1">
-        <v>45540.5335416667</v>
+        <v>45540.5370833333</v>
       </c>
       <c r="C11" s="1">
-        <v>45540.542615740698</v>
+        <v>45540.542870370402</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>76</v>
@@ -2472,88 +2686,88 @@
         <v>73</v>
       </c>
       <c r="G11" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="H11" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="I11" t="s">
-        <v>79</v>
+        <v>58</v>
       </c>
       <c r="J11" t="s">
+        <v>58</v>
+      </c>
+      <c r="K11" t="s">
+        <v>55</v>
+      </c>
+      <c r="L11" t="s">
+        <v>55</v>
+      </c>
+      <c r="M11" t="s">
+        <v>55</v>
+      </c>
+      <c r="N11" t="s">
+        <v>56</v>
+      </c>
+      <c r="O11" t="s">
+        <v>55</v>
+      </c>
+      <c r="P11" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>56</v>
+      </c>
+      <c r="R11" t="s">
+        <v>58</v>
+      </c>
+      <c r="S11" t="s">
+        <v>58</v>
+      </c>
+      <c r="T11" t="s">
+        <v>58</v>
+      </c>
+      <c r="U11" t="s">
         <v>57</v>
       </c>
-      <c r="K11" t="s">
-        <v>54</v>
-      </c>
-      <c r="L11" t="s">
-        <v>54</v>
-      </c>
-      <c r="M11" t="s">
-        <v>55</v>
-      </c>
-      <c r="N11" t="s">
-        <v>55</v>
-      </c>
-      <c r="O11" t="s">
-        <v>54</v>
-      </c>
-      <c r="P11" t="s">
-        <v>54</v>
-      </c>
-      <c r="Q11" t="s">
+      <c r="V11" t="s">
+        <v>55</v>
+      </c>
+      <c r="W11" t="s">
         <v>57</v>
       </c>
-      <c r="R11" t="s">
-        <v>79</v>
-      </c>
-      <c r="S11" t="s">
-        <v>79</v>
-      </c>
-      <c r="T11" t="s">
-        <v>79</v>
-      </c>
-      <c r="U11" t="s">
-        <v>56</v>
-      </c>
-      <c r="V11" t="s">
-        <v>55</v>
-      </c>
-      <c r="W11" t="s">
-        <v>55</v>
-      </c>
       <c r="X11" t="s">
-        <v>79</v>
+        <v>58</v>
       </c>
       <c r="Y11" t="s">
-        <v>79</v>
+        <v>58</v>
       </c>
       <c r="Z11" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="AA11" t="s">
-        <v>79</v>
+        <v>58</v>
       </c>
       <c r="AB11" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="AC11" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="AD11" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="AE11" t="s">
-        <v>79</v>
+        <v>58</v>
       </c>
       <c r="AF11" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="AG11" t="s">
         <v>79</v>
       </c>
       <c r="AH11" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="AI11" t="s">
         <v>56</v>
@@ -2565,147 +2779,141 @@
         <v>74</v>
       </c>
       <c r="AL11" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="AM11" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="AN11" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="AO11" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="AP11" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="AQ11" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="AR11" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="AS11" t="s">
-        <v>79</v>
+        <v>58</v>
       </c>
       <c r="AT11" t="s">
-        <v>79</v>
+        <v>58</v>
       </c>
       <c r="AU11" t="s">
-        <v>79</v>
+        <v>56</v>
       </c>
       <c r="AV11" s="2" t="s">
-        <v>68</v>
+        <v>104</v>
       </c>
       <c r="AW11" t="s">
-        <v>100</v>
-      </c>
-      <c r="AX11" t="s">
-        <v>101</v>
-      </c>
-      <c r="AY11" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
     </row>
     <row r="12" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B12" s="1">
-        <v>45540.537314814799</v>
+        <v>45594.490231481497</v>
       </c>
       <c r="C12" s="1">
-        <v>45540.542638888903</v>
+        <v>45594.494953703703</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="E12" t="s">
-        <v>52</v>
+        <v>107</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="G12" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="H12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I12" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="J12" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="K12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="L12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="M12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="N12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="O12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="P12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="Q12" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="R12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="S12" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="T12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="U12" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="V12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="W12" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="X12" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="Y12" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="Z12" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="AA12" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="AB12" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="AC12" t="s">
-        <v>56</v>
+        <v>79</v>
       </c>
       <c r="AD12" t="s">
         <v>54</v>
       </c>
       <c r="AE12" t="s">
-        <v>58</v>
+        <v>79</v>
       </c>
       <c r="AF12" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="AG12" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="AH12" t="s">
         <v>54</v>
@@ -2714,16 +2922,16 @@
         <v>54</v>
       </c>
       <c r="AJ12" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="AK12" t="s">
-        <v>74</v>
+        <v>59</v>
       </c>
       <c r="AL12" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="AM12" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="AN12" t="s">
         <v>54</v>
@@ -2732,13 +2940,16 @@
         <v>54</v>
       </c>
       <c r="AP12" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="AQ12" t="s">
-        <v>56</v>
+        <v>58</v>
+      </c>
+      <c r="AR12" t="s">
+        <v>109</v>
       </c>
       <c r="AS12" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="AT12" t="s">
         <v>56</v>
@@ -2747,42 +2958,45 @@
         <v>56</v>
       </c>
       <c r="AV12" s="2" t="s">
-        <v>68</v>
+        <v>93</v>
       </c>
       <c r="AW12" t="s">
-        <v>105</v>
+        <v>110</v>
+      </c>
+      <c r="AX12" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="13" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A13">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B13" s="1">
-        <v>45540.5370833333</v>
+        <v>45594.4909259259</v>
       </c>
       <c r="C13" s="1">
-        <v>45540.542870370402</v>
+        <v>45594.498634259297</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>76</v>
+        <v>112</v>
       </c>
       <c r="E13" t="s">
         <v>52</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>73</v>
+        <v>104</v>
       </c>
       <c r="G13" t="s">
         <v>58</v>
       </c>
       <c r="H13" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="I13" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="J13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="K13" t="s">
         <v>55</v>
@@ -2791,37 +3005,37 @@
         <v>55</v>
       </c>
       <c r="M13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="N13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="O13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="P13" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="Q13" t="s">
         <v>56</v>
       </c>
       <c r="R13" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="S13" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="T13" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="U13" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="V13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="W13" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="X13" t="s">
         <v>58</v>
@@ -2836,70 +3050,3077 @@
         <v>58</v>
       </c>
       <c r="AB13" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="AC13" t="s">
         <v>58</v>
       </c>
       <c r="AD13" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="AE13" t="s">
         <v>58</v>
       </c>
       <c r="AF13" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="AG13" t="s">
         <v>79</v>
       </c>
       <c r="AH13" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="AI13" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="AJ13" t="s">
         <v>56</v>
       </c>
       <c r="AK13" t="s">
+        <v>59</v>
+      </c>
+      <c r="AL13" t="s">
+        <v>60</v>
+      </c>
+      <c r="AM13" t="s">
+        <v>56</v>
+      </c>
+      <c r="AN13" t="s">
+        <v>60</v>
+      </c>
+      <c r="AO13" t="s">
+        <v>60</v>
+      </c>
+      <c r="AP13" t="s">
+        <v>79</v>
+      </c>
+      <c r="AQ13" t="s">
+        <v>54</v>
+      </c>
+      <c r="AR13" t="s">
+        <v>113</v>
+      </c>
+      <c r="AS13" t="s">
+        <v>79</v>
+      </c>
+      <c r="AT13" t="s">
+        <v>56</v>
+      </c>
+      <c r="AU13" t="s">
+        <v>56</v>
+      </c>
+      <c r="AV13" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="AW13" t="s">
+        <v>115</v>
+      </c>
+      <c r="AX13" t="s">
+        <v>116</v>
+      </c>
+      <c r="AY13" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="14" spans="1:51" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>16</v>
+      </c>
+      <c r="B14" s="1">
+        <v>45594.490381944401</v>
+      </c>
+      <c r="C14" s="1">
+        <v>45594.498796296299</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="E14" t="s">
+        <v>52</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="G14" t="s">
+        <v>56</v>
+      </c>
+      <c r="H14" t="s">
+        <v>55</v>
+      </c>
+      <c r="I14" t="s">
+        <v>57</v>
+      </c>
+      <c r="J14" t="s">
+        <v>57</v>
+      </c>
+      <c r="K14" t="s">
+        <v>55</v>
+      </c>
+      <c r="L14" t="s">
+        <v>55</v>
+      </c>
+      <c r="M14" t="s">
+        <v>55</v>
+      </c>
+      <c r="N14" t="s">
+        <v>55</v>
+      </c>
+      <c r="O14" t="s">
+        <v>54</v>
+      </c>
+      <c r="P14" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>55</v>
+      </c>
+      <c r="R14" t="s">
+        <v>56</v>
+      </c>
+      <c r="S14" t="s">
+        <v>57</v>
+      </c>
+      <c r="T14" t="s">
+        <v>57</v>
+      </c>
+      <c r="U14" t="s">
+        <v>55</v>
+      </c>
+      <c r="V14" t="s">
+        <v>55</v>
+      </c>
+      <c r="W14" t="s">
+        <v>56</v>
+      </c>
+      <c r="X14" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y14" t="s">
+        <v>56</v>
+      </c>
+      <c r="Z14" t="s">
+        <v>54</v>
+      </c>
+      <c r="AA14" t="s">
+        <v>58</v>
+      </c>
+      <c r="AB14" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC14" t="s">
+        <v>56</v>
+      </c>
+      <c r="AD14" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE14" t="s">
+        <v>58</v>
+      </c>
+      <c r="AF14" t="s">
+        <v>56</v>
+      </c>
+      <c r="AG14" t="s">
+        <v>58</v>
+      </c>
+      <c r="AH14" t="s">
+        <v>54</v>
+      </c>
+      <c r="AI14" t="s">
+        <v>56</v>
+      </c>
+      <c r="AJ14" t="s">
+        <v>56</v>
+      </c>
+      <c r="AK14" t="s">
+        <v>120</v>
+      </c>
+      <c r="AL14" t="s">
+        <v>60</v>
+      </c>
+      <c r="AM14" t="s">
+        <v>54</v>
+      </c>
+      <c r="AN14" t="s">
+        <v>54</v>
+      </c>
+      <c r="AO14" t="s">
+        <v>60</v>
+      </c>
+      <c r="AP14" t="s">
+        <v>56</v>
+      </c>
+      <c r="AQ14" t="s">
+        <v>54</v>
+      </c>
+      <c r="AS14" t="s">
+        <v>56</v>
+      </c>
+      <c r="AT14" t="s">
+        <v>58</v>
+      </c>
+      <c r="AU14" t="s">
+        <v>56</v>
+      </c>
+      <c r="AV14" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="AW14" t="s">
+        <v>122</v>
+      </c>
+      <c r="AX14" t="s">
+        <v>123</v>
+      </c>
+      <c r="AY14" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="15" spans="1:51" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>17</v>
+      </c>
+      <c r="B15" s="1">
+        <v>45594.490532407399</v>
+      </c>
+      <c r="C15" s="1">
+        <v>45594.498946759297</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="E15" t="s">
+        <v>52</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="G15" t="s">
+        <v>58</v>
+      </c>
+      <c r="H15" t="s">
+        <v>56</v>
+      </c>
+      <c r="I15" t="s">
+        <v>58</v>
+      </c>
+      <c r="J15" t="s">
+        <v>58</v>
+      </c>
+      <c r="K15" t="s">
+        <v>55</v>
+      </c>
+      <c r="L15" t="s">
+        <v>55</v>
+      </c>
+      <c r="M15" t="s">
+        <v>55</v>
+      </c>
+      <c r="N15" t="s">
+        <v>55</v>
+      </c>
+      <c r="O15" t="s">
+        <v>56</v>
+      </c>
+      <c r="P15" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>55</v>
+      </c>
+      <c r="R15" t="s">
+        <v>57</v>
+      </c>
+      <c r="S15" t="s">
+        <v>57</v>
+      </c>
+      <c r="T15" t="s">
+        <v>57</v>
+      </c>
+      <c r="U15" t="s">
+        <v>55</v>
+      </c>
+      <c r="V15" t="s">
+        <v>55</v>
+      </c>
+      <c r="W15" t="s">
+        <v>58</v>
+      </c>
+      <c r="X15" t="s">
+        <v>58</v>
+      </c>
+      <c r="Y15" t="s">
+        <v>79</v>
+      </c>
+      <c r="Z15" t="s">
+        <v>54</v>
+      </c>
+      <c r="AA15" t="s">
+        <v>58</v>
+      </c>
+      <c r="AB15" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC15" t="s">
+        <v>79</v>
+      </c>
+      <c r="AD15" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE15" t="s">
+        <v>58</v>
+      </c>
+      <c r="AF15" t="s">
+        <v>54</v>
+      </c>
+      <c r="AG15" t="s">
+        <v>79</v>
+      </c>
+      <c r="AH15" t="s">
+        <v>54</v>
+      </c>
+      <c r="AI15" t="s">
+        <v>56</v>
+      </c>
+      <c r="AJ15" t="s">
+        <v>58</v>
+      </c>
+      <c r="AK15" t="s">
+        <v>59</v>
+      </c>
+      <c r="AL15" t="s">
+        <v>60</v>
+      </c>
+      <c r="AM15" t="s">
+        <v>54</v>
+      </c>
+      <c r="AN15" t="s">
+        <v>54</v>
+      </c>
+      <c r="AO15" t="s">
+        <v>60</v>
+      </c>
+      <c r="AP15" t="s">
+        <v>54</v>
+      </c>
+      <c r="AQ15" t="s">
+        <v>54</v>
+      </c>
+      <c r="AR15" t="s">
+        <v>126</v>
+      </c>
+      <c r="AS15" t="s">
+        <v>58</v>
+      </c>
+      <c r="AT15" t="s">
+        <v>56</v>
+      </c>
+      <c r="AU15" t="s">
+        <v>58</v>
+      </c>
+      <c r="AV15" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="AW15" t="s">
+        <v>127</v>
+      </c>
+      <c r="AY15" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="16" spans="1:51" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>18</v>
+      </c>
+      <c r="B16" s="1">
+        <v>45594.491747685199</v>
+      </c>
+      <c r="C16" s="1">
+        <v>45594.4999074074</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="E16" t="s">
+        <v>52</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="G16" t="s">
+        <v>58</v>
+      </c>
+      <c r="H16" t="s">
+        <v>55</v>
+      </c>
+      <c r="I16" t="s">
+        <v>55</v>
+      </c>
+      <c r="J16" t="s">
+        <v>55</v>
+      </c>
+      <c r="K16" t="s">
+        <v>54</v>
+      </c>
+      <c r="L16" t="s">
+        <v>54</v>
+      </c>
+      <c r="M16" t="s">
+        <v>54</v>
+      </c>
+      <c r="N16" t="s">
+        <v>54</v>
+      </c>
+      <c r="O16" t="s">
+        <v>54</v>
+      </c>
+      <c r="P16" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>56</v>
+      </c>
+      <c r="R16" t="s">
+        <v>55</v>
+      </c>
+      <c r="S16" t="s">
+        <v>55</v>
+      </c>
+      <c r="T16" t="s">
+        <v>55</v>
+      </c>
+      <c r="U16" t="s">
+        <v>55</v>
+      </c>
+      <c r="V16" t="s">
+        <v>54</v>
+      </c>
+      <c r="W16" t="s">
+        <v>56</v>
+      </c>
+      <c r="X16" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y16" t="s">
+        <v>79</v>
+      </c>
+      <c r="Z16" t="s">
+        <v>60</v>
+      </c>
+      <c r="AA16" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB16" t="s">
+        <v>60</v>
+      </c>
+      <c r="AC16" t="s">
+        <v>79</v>
+      </c>
+      <c r="AD16" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE16" t="s">
+        <v>79</v>
+      </c>
+      <c r="AF16" t="s">
+        <v>54</v>
+      </c>
+      <c r="AG16" t="s">
+        <v>79</v>
+      </c>
+      <c r="AH16" t="s">
+        <v>54</v>
+      </c>
+      <c r="AI16" t="s">
+        <v>56</v>
+      </c>
+      <c r="AJ16" t="s">
+        <v>56</v>
+      </c>
+      <c r="AK16" t="s">
+        <v>59</v>
+      </c>
+      <c r="AL16" t="s">
+        <v>54</v>
+      </c>
+      <c r="AM16" t="s">
+        <v>54</v>
+      </c>
+      <c r="AN16" t="s">
+        <v>60</v>
+      </c>
+      <c r="AO16" t="s">
+        <v>60</v>
+      </c>
+      <c r="AP16" t="s">
+        <v>54</v>
+      </c>
+      <c r="AQ16" t="s">
+        <v>54</v>
+      </c>
+      <c r="AR16" t="s">
+        <v>130</v>
+      </c>
+      <c r="AS16" t="s">
+        <v>58</v>
+      </c>
+      <c r="AT16" t="s">
+        <v>56</v>
+      </c>
+      <c r="AU16" t="s">
+        <v>58</v>
+      </c>
+      <c r="AV16" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="AW16" t="s">
+        <v>131</v>
+      </c>
+      <c r="AY16" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="17" spans="1:51" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>19</v>
+      </c>
+      <c r="B17" s="1">
+        <v>45607.562719907401</v>
+      </c>
+      <c r="C17" s="1">
+        <v>45607.568229166704</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="E17" t="s">
+        <v>52</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="G17" t="s">
+        <v>58</v>
+      </c>
+      <c r="H17" t="s">
+        <v>57</v>
+      </c>
+      <c r="I17" t="s">
+        <v>55</v>
+      </c>
+      <c r="J17" t="s">
+        <v>57</v>
+      </c>
+      <c r="K17" t="s">
+        <v>55</v>
+      </c>
+      <c r="L17" t="s">
+        <v>55</v>
+      </c>
+      <c r="M17" t="s">
+        <v>54</v>
+      </c>
+      <c r="N17" t="s">
+        <v>55</v>
+      </c>
+      <c r="O17" t="s">
+        <v>55</v>
+      </c>
+      <c r="P17" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>56</v>
+      </c>
+      <c r="R17" t="s">
+        <v>56</v>
+      </c>
+      <c r="S17" t="s">
+        <v>55</v>
+      </c>
+      <c r="T17" t="s">
+        <v>56</v>
+      </c>
+      <c r="U17" t="s">
+        <v>54</v>
+      </c>
+      <c r="V17" t="s">
+        <v>55</v>
+      </c>
+      <c r="W17" t="s">
+        <v>55</v>
+      </c>
+      <c r="X17" t="s">
+        <v>58</v>
+      </c>
+      <c r="Y17" t="s">
+        <v>58</v>
+      </c>
+      <c r="Z17" t="s">
+        <v>54</v>
+      </c>
+      <c r="AA17" t="s">
+        <v>58</v>
+      </c>
+      <c r="AB17" t="s">
+        <v>56</v>
+      </c>
+      <c r="AC17" t="s">
+        <v>58</v>
+      </c>
+      <c r="AD17" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE17" t="s">
+        <v>58</v>
+      </c>
+      <c r="AF17" t="s">
+        <v>54</v>
+      </c>
+      <c r="AG17" t="s">
+        <v>58</v>
+      </c>
+      <c r="AH17" t="s">
+        <v>54</v>
+      </c>
+      <c r="AI17" t="s">
+        <v>54</v>
+      </c>
+      <c r="AJ17" t="s">
+        <v>54</v>
+      </c>
+      <c r="AK17" t="s">
+        <v>59</v>
+      </c>
+      <c r="AL17" t="s">
+        <v>60</v>
+      </c>
+      <c r="AM17" t="s">
+        <v>60</v>
+      </c>
+      <c r="AN17" t="s">
+        <v>60</v>
+      </c>
+      <c r="AO17" t="s">
+        <v>60</v>
+      </c>
+      <c r="AP17" t="s">
+        <v>60</v>
+      </c>
+      <c r="AQ17" t="s">
+        <v>60</v>
+      </c>
+      <c r="AS17" t="s">
+        <v>58</v>
+      </c>
+      <c r="AT17" t="s">
+        <v>56</v>
+      </c>
+      <c r="AU17" t="s">
+        <v>58</v>
+      </c>
+      <c r="AV17" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="18" spans="1:51" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>20</v>
+      </c>
+      <c r="B18" s="1">
+        <v>45607.5715740741</v>
+      </c>
+      <c r="C18" s="1">
+        <v>45607.575185185196</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="E18" t="s">
+        <v>52</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="G18" t="s">
+        <v>58</v>
+      </c>
+      <c r="H18" t="s">
+        <v>54</v>
+      </c>
+      <c r="I18" t="s">
+        <v>54</v>
+      </c>
+      <c r="J18" t="s">
+        <v>54</v>
+      </c>
+      <c r="K18" t="s">
+        <v>54</v>
+      </c>
+      <c r="L18" t="s">
+        <v>54</v>
+      </c>
+      <c r="M18" t="s">
+        <v>54</v>
+      </c>
+      <c r="N18" t="s">
+        <v>54</v>
+      </c>
+      <c r="O18" t="s">
+        <v>54</v>
+      </c>
+      <c r="P18" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>54</v>
+      </c>
+      <c r="R18" t="s">
+        <v>54</v>
+      </c>
+      <c r="S18" t="s">
+        <v>54</v>
+      </c>
+      <c r="T18" t="s">
+        <v>54</v>
+      </c>
+      <c r="U18" t="s">
+        <v>54</v>
+      </c>
+      <c r="V18" t="s">
+        <v>54</v>
+      </c>
+      <c r="W18" t="s">
+        <v>55</v>
+      </c>
+      <c r="X18" t="s">
+        <v>54</v>
+      </c>
+      <c r="Y18" t="s">
+        <v>58</v>
+      </c>
+      <c r="Z18" t="s">
+        <v>54</v>
+      </c>
+      <c r="AA18" t="s">
+        <v>58</v>
+      </c>
+      <c r="AB18" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC18" t="s">
+        <v>58</v>
+      </c>
+      <c r="AD18" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE18" t="s">
+        <v>58</v>
+      </c>
+      <c r="AF18" t="s">
+        <v>54</v>
+      </c>
+      <c r="AG18" t="s">
+        <v>58</v>
+      </c>
+      <c r="AH18" t="s">
+        <v>56</v>
+      </c>
+      <c r="AI18" t="s">
+        <v>54</v>
+      </c>
+      <c r="AJ18" t="s">
+        <v>54</v>
+      </c>
+      <c r="AK18" t="s">
+        <v>59</v>
+      </c>
+      <c r="AL18" t="s">
+        <v>58</v>
+      </c>
+      <c r="AM18" t="s">
+        <v>54</v>
+      </c>
+      <c r="AN18" t="s">
+        <v>60</v>
+      </c>
+      <c r="AO18" t="s">
+        <v>60</v>
+      </c>
+      <c r="AP18" t="s">
+        <v>54</v>
+      </c>
+      <c r="AQ18" t="s">
+        <v>54</v>
+      </c>
+      <c r="AS18" t="s">
+        <v>56</v>
+      </c>
+      <c r="AT18" t="s">
+        <v>56</v>
+      </c>
+      <c r="AU18" t="s">
+        <v>58</v>
+      </c>
+      <c r="AV18" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="AW18" t="s">
+        <v>135</v>
+      </c>
+      <c r="AX18" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="AY18" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="19" spans="1:51" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>21</v>
+      </c>
+      <c r="B19" s="1">
+        <v>45607.573263888902</v>
+      </c>
+      <c r="C19" s="1">
+        <v>45607.576516203699</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="E19" t="s">
+        <v>52</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="G19" t="s">
+        <v>58</v>
+      </c>
+      <c r="H19" t="s">
+        <v>55</v>
+      </c>
+      <c r="I19" t="s">
+        <v>57</v>
+      </c>
+      <c r="J19" t="s">
+        <v>57</v>
+      </c>
+      <c r="K19" t="s">
+        <v>55</v>
+      </c>
+      <c r="L19" t="s">
+        <v>55</v>
+      </c>
+      <c r="M19" t="s">
+        <v>55</v>
+      </c>
+      <c r="N19" t="s">
+        <v>55</v>
+      </c>
+      <c r="O19" t="s">
+        <v>55</v>
+      </c>
+      <c r="P19" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>56</v>
+      </c>
+      <c r="R19" t="s">
+        <v>57</v>
+      </c>
+      <c r="S19" t="s">
+        <v>57</v>
+      </c>
+      <c r="T19" t="s">
+        <v>57</v>
+      </c>
+      <c r="U19" t="s">
+        <v>55</v>
+      </c>
+      <c r="V19" t="s">
+        <v>54</v>
+      </c>
+      <c r="W19" t="s">
+        <v>55</v>
+      </c>
+      <c r="X19" t="s">
+        <v>58</v>
+      </c>
+      <c r="Y19" t="s">
+        <v>58</v>
+      </c>
+      <c r="Z19" t="s">
+        <v>54</v>
+      </c>
+      <c r="AA19" t="s">
+        <v>58</v>
+      </c>
+      <c r="AB19" t="s">
+        <v>79</v>
+      </c>
+      <c r="AC19" t="s">
+        <v>56</v>
+      </c>
+      <c r="AD19" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE19" t="s">
+        <v>58</v>
+      </c>
+      <c r="AF19" t="s">
+        <v>58</v>
+      </c>
+      <c r="AG19" t="s">
+        <v>58</v>
+      </c>
+      <c r="AH19" t="s">
+        <v>54</v>
+      </c>
+      <c r="AI19" t="s">
+        <v>58</v>
+      </c>
+      <c r="AJ19" t="s">
+        <v>58</v>
+      </c>
+      <c r="AK19" t="s">
+        <v>59</v>
+      </c>
+      <c r="AL19" t="s">
+        <v>60</v>
+      </c>
+      <c r="AM19" t="s">
+        <v>60</v>
+      </c>
+      <c r="AN19" t="s">
+        <v>60</v>
+      </c>
+      <c r="AO19" t="s">
+        <v>60</v>
+      </c>
+      <c r="AP19" t="s">
+        <v>60</v>
+      </c>
+      <c r="AQ19" t="s">
+        <v>60</v>
+      </c>
+      <c r="AS19" t="s">
+        <v>58</v>
+      </c>
+      <c r="AT19" t="s">
+        <v>58</v>
+      </c>
+      <c r="AU19" t="s">
+        <v>79</v>
+      </c>
+      <c r="AV19" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="20" spans="1:51" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>22</v>
+      </c>
+      <c r="B20" s="1">
+        <v>45607.572268518503</v>
+      </c>
+      <c r="C20" s="1">
+        <v>45607.576701388898</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="E20" t="s">
+        <v>52</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="G20" t="s">
+        <v>56</v>
+      </c>
+      <c r="H20" t="s">
+        <v>55</v>
+      </c>
+      <c r="I20" t="s">
+        <v>56</v>
+      </c>
+      <c r="J20" t="s">
+        <v>56</v>
+      </c>
+      <c r="K20" t="s">
+        <v>54</v>
+      </c>
+      <c r="L20" t="s">
+        <v>55</v>
+      </c>
+      <c r="M20" t="s">
+        <v>55</v>
+      </c>
+      <c r="N20" t="s">
+        <v>55</v>
+      </c>
+      <c r="O20" t="s">
+        <v>55</v>
+      </c>
+      <c r="P20" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>55</v>
+      </c>
+      <c r="R20" t="s">
+        <v>55</v>
+      </c>
+      <c r="S20" t="s">
+        <v>55</v>
+      </c>
+      <c r="T20" t="s">
+        <v>55</v>
+      </c>
+      <c r="U20" t="s">
+        <v>55</v>
+      </c>
+      <c r="V20" t="s">
+        <v>55</v>
+      </c>
+      <c r="W20" t="s">
+        <v>54</v>
+      </c>
+      <c r="X20" t="s">
+        <v>54</v>
+      </c>
+      <c r="Y20" t="s">
+        <v>56</v>
+      </c>
+      <c r="Z20" t="s">
+        <v>54</v>
+      </c>
+      <c r="AA20" t="s">
+        <v>58</v>
+      </c>
+      <c r="AB20" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC20" t="s">
+        <v>58</v>
+      </c>
+      <c r="AD20" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE20" t="s">
+        <v>58</v>
+      </c>
+      <c r="AF20" t="s">
+        <v>54</v>
+      </c>
+      <c r="AG20" t="s">
+        <v>58</v>
+      </c>
+      <c r="AH20" t="s">
+        <v>56</v>
+      </c>
+      <c r="AI20" t="s">
+        <v>54</v>
+      </c>
+      <c r="AJ20" t="s">
+        <v>54</v>
+      </c>
+      <c r="AK20" t="s">
+        <v>120</v>
+      </c>
+      <c r="AL20" t="s">
+        <v>54</v>
+      </c>
+      <c r="AM20" t="s">
+        <v>54</v>
+      </c>
+      <c r="AN20" t="s">
+        <v>54</v>
+      </c>
+      <c r="AO20" t="s">
+        <v>54</v>
+      </c>
+      <c r="AP20" t="s">
+        <v>56</v>
+      </c>
+      <c r="AQ20" t="s">
+        <v>56</v>
+      </c>
+      <c r="AS20" t="s">
+        <v>56</v>
+      </c>
+      <c r="AT20" t="s">
+        <v>56</v>
+      </c>
+      <c r="AU20" t="s">
+        <v>56</v>
+      </c>
+      <c r="AV20" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="AW20" t="s">
+        <v>136</v>
+      </c>
+      <c r="AX20" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="21" spans="1:51" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>23</v>
+      </c>
+      <c r="B21" s="1">
+        <v>45607.571516203701</v>
+      </c>
+      <c r="C21" s="1">
+        <v>45607.577384259297</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="E21" t="s">
+        <v>52</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G21" t="s">
+        <v>54</v>
+      </c>
+      <c r="H21" t="s">
+        <v>55</v>
+      </c>
+      <c r="I21" t="s">
+        <v>55</v>
+      </c>
+      <c r="J21" t="s">
+        <v>55</v>
+      </c>
+      <c r="K21" t="s">
+        <v>55</v>
+      </c>
+      <c r="L21" t="s">
+        <v>55</v>
+      </c>
+      <c r="M21" t="s">
+        <v>55</v>
+      </c>
+      <c r="N21" t="s">
+        <v>55</v>
+      </c>
+      <c r="O21" t="s">
+        <v>57</v>
+      </c>
+      <c r="P21" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>55</v>
+      </c>
+      <c r="R21" t="s">
+        <v>55</v>
+      </c>
+      <c r="S21" t="s">
+        <v>55</v>
+      </c>
+      <c r="T21" t="s">
+        <v>55</v>
+      </c>
+      <c r="U21" t="s">
+        <v>54</v>
+      </c>
+      <c r="V21" t="s">
+        <v>54</v>
+      </c>
+      <c r="W21" t="s">
+        <v>54</v>
+      </c>
+      <c r="X21" t="s">
+        <v>54</v>
+      </c>
+      <c r="Y21" t="s">
+        <v>58</v>
+      </c>
+      <c r="Z21" t="s">
+        <v>54</v>
+      </c>
+      <c r="AA21" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB21" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC21" t="s">
+        <v>58</v>
+      </c>
+      <c r="AD21" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE21" t="s">
+        <v>58</v>
+      </c>
+      <c r="AF21" t="s">
+        <v>54</v>
+      </c>
+      <c r="AG21" t="s">
+        <v>79</v>
+      </c>
+      <c r="AH21" t="s">
+        <v>54</v>
+      </c>
+      <c r="AI21" t="s">
+        <v>54</v>
+      </c>
+      <c r="AJ21" t="s">
+        <v>54</v>
+      </c>
+      <c r="AK21" t="s">
+        <v>120</v>
+      </c>
+      <c r="AL21" t="s">
+        <v>58</v>
+      </c>
+      <c r="AM21" t="s">
+        <v>60</v>
+      </c>
+      <c r="AN21" t="s">
+        <v>60</v>
+      </c>
+      <c r="AO21" t="s">
+        <v>60</v>
+      </c>
+      <c r="AP21" t="s">
+        <v>60</v>
+      </c>
+      <c r="AQ21" t="s">
+        <v>60</v>
+      </c>
+      <c r="AS21" t="s">
+        <v>54</v>
+      </c>
+      <c r="AT21" t="s">
+        <v>54</v>
+      </c>
+      <c r="AU21" t="s">
+        <v>54</v>
+      </c>
+      <c r="AV21" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="AW21" t="s">
+        <v>140</v>
+      </c>
+      <c r="AY21" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="22" spans="1:51" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>24</v>
+      </c>
+      <c r="B22" s="1">
+        <v>45607.572881944398</v>
+      </c>
+      <c r="C22" s="1">
+        <v>45607.577928240702</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="E22" t="s">
+        <v>52</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="G22" t="s">
+        <v>54</v>
+      </c>
+      <c r="H22" t="s">
+        <v>55</v>
+      </c>
+      <c r="I22" t="s">
+        <v>55</v>
+      </c>
+      <c r="J22" t="s">
+        <v>55</v>
+      </c>
+      <c r="K22" t="s">
+        <v>54</v>
+      </c>
+      <c r="L22" t="s">
+        <v>54</v>
+      </c>
+      <c r="M22" t="s">
+        <v>54</v>
+      </c>
+      <c r="N22" t="s">
+        <v>55</v>
+      </c>
+      <c r="O22" t="s">
+        <v>54</v>
+      </c>
+      <c r="P22" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>56</v>
+      </c>
+      <c r="R22" t="s">
+        <v>55</v>
+      </c>
+      <c r="S22" t="s">
+        <v>55</v>
+      </c>
+      <c r="T22" t="s">
+        <v>55</v>
+      </c>
+      <c r="U22" t="s">
+        <v>55</v>
+      </c>
+      <c r="V22" t="s">
+        <v>55</v>
+      </c>
+      <c r="W22" t="s">
+        <v>55</v>
+      </c>
+      <c r="X22" t="s">
+        <v>54</v>
+      </c>
+      <c r="Y22" t="s">
+        <v>79</v>
+      </c>
+      <c r="Z22" t="s">
+        <v>60</v>
+      </c>
+      <c r="AA22" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB22" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC22" t="s">
+        <v>79</v>
+      </c>
+      <c r="AD22" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE22" t="s">
+        <v>79</v>
+      </c>
+      <c r="AF22" t="s">
+        <v>54</v>
+      </c>
+      <c r="AG22" t="s">
+        <v>79</v>
+      </c>
+      <c r="AH22" t="s">
+        <v>54</v>
+      </c>
+      <c r="AI22" t="s">
+        <v>54</v>
+      </c>
+      <c r="AJ22" t="s">
+        <v>54</v>
+      </c>
+      <c r="AK22" t="s">
+        <v>120</v>
+      </c>
+      <c r="AL22" t="s">
+        <v>60</v>
+      </c>
+      <c r="AM22" t="s">
+        <v>54</v>
+      </c>
+      <c r="AN22" t="s">
+        <v>54</v>
+      </c>
+      <c r="AO22" t="s">
+        <v>56</v>
+      </c>
+      <c r="AP22" t="s">
+        <v>60</v>
+      </c>
+      <c r="AQ22" t="s">
+        <v>60</v>
+      </c>
+      <c r="AS22" t="s">
+        <v>56</v>
+      </c>
+      <c r="AT22" t="s">
+        <v>54</v>
+      </c>
+      <c r="AU22" t="s">
+        <v>56</v>
+      </c>
+      <c r="AV22" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="AW22" t="s">
+        <v>144</v>
+      </c>
+      <c r="AX22" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="23" spans="1:51" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>25</v>
+      </c>
+      <c r="B23" s="1">
+        <v>45607.571678240703</v>
+      </c>
+      <c r="C23" s="1">
+        <v>45607.578750000001</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="E23" t="s">
+        <v>52</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="G23" t="s">
+        <v>58</v>
+      </c>
+      <c r="H23" t="s">
+        <v>56</v>
+      </c>
+      <c r="I23" t="s">
+        <v>58</v>
+      </c>
+      <c r="J23" t="s">
+        <v>58</v>
+      </c>
+      <c r="K23" t="s">
+        <v>56</v>
+      </c>
+      <c r="L23" t="s">
+        <v>56</v>
+      </c>
+      <c r="M23" t="s">
+        <v>56</v>
+      </c>
+      <c r="N23" t="s">
+        <v>57</v>
+      </c>
+      <c r="O23" t="s">
+        <v>56</v>
+      </c>
+      <c r="P23" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>56</v>
+      </c>
+      <c r="R23" t="s">
+        <v>57</v>
+      </c>
+      <c r="S23" t="s">
+        <v>57</v>
+      </c>
+      <c r="T23" t="s">
+        <v>57</v>
+      </c>
+      <c r="U23" t="s">
+        <v>56</v>
+      </c>
+      <c r="V23" t="s">
+        <v>56</v>
+      </c>
+      <c r="W23" t="s">
+        <v>56</v>
+      </c>
+      <c r="X23" t="s">
+        <v>58</v>
+      </c>
+      <c r="Y23" t="s">
+        <v>56</v>
+      </c>
+      <c r="Z23" t="s">
+        <v>56</v>
+      </c>
+      <c r="AA23" t="s">
+        <v>56</v>
+      </c>
+      <c r="AB23" t="s">
+        <v>56</v>
+      </c>
+      <c r="AC23" t="s">
+        <v>56</v>
+      </c>
+      <c r="AD23" t="s">
+        <v>56</v>
+      </c>
+      <c r="AE23" t="s">
+        <v>54</v>
+      </c>
+      <c r="AF23" t="s">
+        <v>58</v>
+      </c>
+      <c r="AG23" t="s">
+        <v>56</v>
+      </c>
+      <c r="AH23" t="s">
+        <v>56</v>
+      </c>
+      <c r="AI23" t="s">
+        <v>56</v>
+      </c>
+      <c r="AJ23" t="s">
+        <v>56</v>
+      </c>
+      <c r="AK23" t="s">
         <v>74</v>
       </c>
-      <c r="AL13" t="s">
-        <v>58</v>
-      </c>
-      <c r="AM13" t="s">
-        <v>58</v>
-      </c>
-      <c r="AN13" t="s">
-        <v>58</v>
-      </c>
-      <c r="AO13" t="s">
-        <v>58</v>
-      </c>
-      <c r="AP13" t="s">
-        <v>58</v>
-      </c>
-      <c r="AQ13" t="s">
-        <v>58</v>
-      </c>
-      <c r="AR13" t="s">
-        <v>106</v>
-      </c>
-      <c r="AS13" t="s">
-        <v>58</v>
-      </c>
-      <c r="AT13" t="s">
-        <v>58</v>
-      </c>
-      <c r="AU13" t="s">
-        <v>56</v>
-      </c>
-      <c r="AV13" s="2" t="s">
+      <c r="AL23" t="s">
+        <v>54</v>
+      </c>
+      <c r="AM23" t="s">
+        <v>54</v>
+      </c>
+      <c r="AN23" t="s">
+        <v>54</v>
+      </c>
+      <c r="AO23" t="s">
+        <v>54</v>
+      </c>
+      <c r="AP23" t="s">
+        <v>54</v>
+      </c>
+      <c r="AQ23" t="s">
+        <v>54</v>
+      </c>
+      <c r="AS23" t="s">
+        <v>56</v>
+      </c>
+      <c r="AT23" t="s">
+        <v>56</v>
+      </c>
+      <c r="AU23" t="s">
+        <v>56</v>
+      </c>
+      <c r="AV23" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="AW23" t="s">
+        <v>147</v>
+      </c>
+      <c r="AX23" t="s">
+        <v>148</v>
+      </c>
+      <c r="AY23" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="24" spans="1:51" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>26</v>
+      </c>
+      <c r="B24" s="1">
+        <v>45607.573275463001</v>
+      </c>
+      <c r="C24" s="1">
+        <v>45607.579641203702</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="E24" t="s">
+        <v>52</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="G24" t="s">
+        <v>58</v>
+      </c>
+      <c r="H24" t="s">
+        <v>55</v>
+      </c>
+      <c r="I24" t="s">
+        <v>56</v>
+      </c>
+      <c r="J24" t="s">
+        <v>56</v>
+      </c>
+      <c r="K24" t="s">
+        <v>55</v>
+      </c>
+      <c r="L24" t="s">
+        <v>55</v>
+      </c>
+      <c r="M24" t="s">
+        <v>55</v>
+      </c>
+      <c r="N24" t="s">
+        <v>55</v>
+      </c>
+      <c r="O24" t="s">
+        <v>55</v>
+      </c>
+      <c r="P24" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>55</v>
+      </c>
+      <c r="R24" t="s">
+        <v>55</v>
+      </c>
+      <c r="S24" t="s">
+        <v>55</v>
+      </c>
+      <c r="T24" t="s">
+        <v>56</v>
+      </c>
+      <c r="U24" t="s">
+        <v>55</v>
+      </c>
+      <c r="V24" t="s">
+        <v>55</v>
+      </c>
+      <c r="W24" t="s">
+        <v>55</v>
+      </c>
+      <c r="X24" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y24" t="s">
+        <v>58</v>
+      </c>
+      <c r="Z24" t="s">
+        <v>54</v>
+      </c>
+      <c r="AA24" t="s">
+        <v>58</v>
+      </c>
+      <c r="AB24" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC24" t="s">
+        <v>56</v>
+      </c>
+      <c r="AD24" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE24" t="s">
+        <v>58</v>
+      </c>
+      <c r="AF24" t="s">
+        <v>54</v>
+      </c>
+      <c r="AG24" t="s">
+        <v>58</v>
+      </c>
+      <c r="AH24" t="s">
+        <v>54</v>
+      </c>
+      <c r="AI24" t="s">
+        <v>54</v>
+      </c>
+      <c r="AJ24" t="s">
+        <v>54</v>
+      </c>
+      <c r="AK24" t="s">
+        <v>59</v>
+      </c>
+      <c r="AL24" t="s">
+        <v>60</v>
+      </c>
+      <c r="AM24" t="s">
+        <v>60</v>
+      </c>
+      <c r="AN24" t="s">
+        <v>60</v>
+      </c>
+      <c r="AO24" t="s">
+        <v>60</v>
+      </c>
+      <c r="AP24" t="s">
+        <v>54</v>
+      </c>
+      <c r="AQ24" t="s">
+        <v>54</v>
+      </c>
+      <c r="AS24" t="s">
+        <v>56</v>
+      </c>
+      <c r="AT24" t="s">
+        <v>56</v>
+      </c>
+      <c r="AU24" t="s">
+        <v>56</v>
+      </c>
+      <c r="AV24" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="AW24" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="25" spans="1:51" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>27</v>
+      </c>
+      <c r="B25" s="1">
+        <v>45607.574583333299</v>
+      </c>
+      <c r="C25" s="1">
+        <v>45607.580960648098</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="E25" t="s">
+        <v>52</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="G25" t="s">
+        <v>54</v>
+      </c>
+      <c r="H25" t="s">
+        <v>54</v>
+      </c>
+      <c r="I25" t="s">
+        <v>56</v>
+      </c>
+      <c r="J25" t="s">
+        <v>55</v>
+      </c>
+      <c r="K25" t="s">
+        <v>60</v>
+      </c>
+      <c r="L25" t="s">
+        <v>60</v>
+      </c>
+      <c r="M25" t="s">
+        <v>60</v>
+      </c>
+      <c r="N25" t="s">
+        <v>60</v>
+      </c>
+      <c r="O25" t="s">
+        <v>55</v>
+      </c>
+      <c r="P25" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q25" t="s">
+        <v>54</v>
+      </c>
+      <c r="R25" t="s">
+        <v>54</v>
+      </c>
+      <c r="S25" t="s">
+        <v>55</v>
+      </c>
+      <c r="T25" t="s">
+        <v>55</v>
+      </c>
+      <c r="U25" t="s">
+        <v>54</v>
+      </c>
+      <c r="V25" t="s">
+        <v>54</v>
+      </c>
+      <c r="W25" t="s">
+        <v>54</v>
+      </c>
+      <c r="X25" t="s">
+        <v>54</v>
+      </c>
+      <c r="Y25" t="s">
+        <v>79</v>
+      </c>
+      <c r="Z25" t="s">
+        <v>60</v>
+      </c>
+      <c r="AA25" t="s">
+        <v>58</v>
+      </c>
+      <c r="AB25" t="s">
+        <v>60</v>
+      </c>
+      <c r="AC25" t="s">
+        <v>79</v>
+      </c>
+      <c r="AD25" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE25" t="s">
+        <v>79</v>
+      </c>
+      <c r="AF25" t="s">
+        <v>54</v>
+      </c>
+      <c r="AG25" t="s">
+        <v>79</v>
+      </c>
+      <c r="AH25" t="s">
+        <v>60</v>
+      </c>
+      <c r="AI25" t="s">
+        <v>54</v>
+      </c>
+      <c r="AJ25" t="s">
+        <v>56</v>
+      </c>
+      <c r="AK25" t="s">
+        <v>120</v>
+      </c>
+      <c r="AL25" t="s">
+        <v>54</v>
+      </c>
+      <c r="AM25" t="s">
+        <v>54</v>
+      </c>
+      <c r="AN25" t="s">
+        <v>54</v>
+      </c>
+      <c r="AO25" t="s">
+        <v>54</v>
+      </c>
+      <c r="AP25" t="s">
+        <v>54</v>
+      </c>
+      <c r="AQ25" t="s">
+        <v>54</v>
+      </c>
+      <c r="AR25" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="AS25" t="s">
+        <v>54</v>
+      </c>
+      <c r="AT25" t="s">
+        <v>54</v>
+      </c>
+      <c r="AU25" t="s">
+        <v>54</v>
+      </c>
+      <c r="AV25" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="AW25" t="s">
+        <v>152</v>
+      </c>
+      <c r="AX25" t="s">
+        <v>153</v>
+      </c>
+      <c r="AY25" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="26" spans="1:51" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>28</v>
+      </c>
+      <c r="B26" s="1">
+        <v>45607.574270833298</v>
+      </c>
+      <c r="C26" s="1">
+        <v>45607.580995370401</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E26" t="s">
+        <v>52</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="G26" t="s">
+        <v>156</v>
+      </c>
+      <c r="H26" t="s">
+        <v>55</v>
+      </c>
+      <c r="I26" t="s">
+        <v>56</v>
+      </c>
+      <c r="J26" t="s">
+        <v>56</v>
+      </c>
+      <c r="K26" t="s">
+        <v>55</v>
+      </c>
+      <c r="L26" t="s">
+        <v>55</v>
+      </c>
+      <c r="M26" t="s">
+        <v>54</v>
+      </c>
+      <c r="N26" t="s">
+        <v>55</v>
+      </c>
+      <c r="O26" t="s">
+        <v>56</v>
+      </c>
+      <c r="P26" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q26" t="s">
+        <v>54</v>
+      </c>
+      <c r="R26" t="s">
+        <v>55</v>
+      </c>
+      <c r="S26" t="s">
+        <v>55</v>
+      </c>
+      <c r="T26" t="s">
+        <v>56</v>
+      </c>
+      <c r="U26" t="s">
+        <v>54</v>
+      </c>
+      <c r="V26" t="s">
+        <v>54</v>
+      </c>
+      <c r="W26" t="s">
+        <v>54</v>
+      </c>
+      <c r="X26" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y26" t="s">
+        <v>58</v>
+      </c>
+      <c r="Z26" t="s">
+        <v>54</v>
+      </c>
+      <c r="AA26" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB26" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC26" t="s">
+        <v>79</v>
+      </c>
+      <c r="AD26" t="s">
+        <v>56</v>
+      </c>
+      <c r="AE26" t="s">
+        <v>56</v>
+      </c>
+      <c r="AF26" t="s">
+        <v>56</v>
+      </c>
+      <c r="AG26" t="s">
+        <v>54</v>
+      </c>
+      <c r="AH26" t="s">
+        <v>60</v>
+      </c>
+      <c r="AI26" t="s">
+        <v>60</v>
+      </c>
+      <c r="AJ26" t="s">
+        <v>54</v>
+      </c>
+      <c r="AK26" t="s">
+        <v>59</v>
+      </c>
+      <c r="AL26" t="s">
+        <v>54</v>
+      </c>
+      <c r="AM26" t="s">
+        <v>60</v>
+      </c>
+      <c r="AN26" t="s">
+        <v>60</v>
+      </c>
+      <c r="AO26" t="s">
+        <v>60</v>
+      </c>
+      <c r="AP26" t="s">
+        <v>60</v>
+      </c>
+      <c r="AQ26" t="s">
+        <v>54</v>
+      </c>
+      <c r="AR26" t="s">
+        <v>157</v>
+      </c>
+      <c r="AS26" t="s">
+        <v>60</v>
+      </c>
+      <c r="AT26" t="s">
+        <v>54</v>
+      </c>
+      <c r="AU26" t="s">
+        <v>60</v>
+      </c>
+      <c r="AV26" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="AW26" t="s">
+        <v>158</v>
+      </c>
+      <c r="AX26" t="s">
+        <v>159</v>
+      </c>
+      <c r="AY26" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="27" spans="1:51" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>29</v>
+      </c>
+      <c r="B27" s="1">
+        <v>45607.574629629598</v>
+      </c>
+      <c r="C27" s="1">
+        <v>45607.583043981504</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="E27" t="s">
+        <v>52</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="G27" t="s">
+        <v>54</v>
+      </c>
+      <c r="H27" t="s">
+        <v>55</v>
+      </c>
+      <c r="I27" t="s">
+        <v>57</v>
+      </c>
+      <c r="J27" t="s">
+        <v>56</v>
+      </c>
+      <c r="K27" t="s">
+        <v>55</v>
+      </c>
+      <c r="L27" t="s">
+        <v>54</v>
+      </c>
+      <c r="M27" t="s">
+        <v>54</v>
+      </c>
+      <c r="N27" t="s">
+        <v>55</v>
+      </c>
+      <c r="O27" t="s">
+        <v>55</v>
+      </c>
+      <c r="P27" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q27" t="s">
+        <v>56</v>
+      </c>
+      <c r="R27" t="s">
+        <v>54</v>
+      </c>
+      <c r="S27" t="s">
+        <v>54</v>
+      </c>
+      <c r="T27" t="s">
+        <v>54</v>
+      </c>
+      <c r="U27" t="s">
+        <v>55</v>
+      </c>
+      <c r="V27" t="s">
+        <v>55</v>
+      </c>
+      <c r="W27" t="s">
+        <v>54</v>
+      </c>
+      <c r="X27" t="s">
+        <v>54</v>
+      </c>
+      <c r="Y27" t="s">
+        <v>58</v>
+      </c>
+      <c r="Z27" t="s">
+        <v>54</v>
+      </c>
+      <c r="AA27" t="s">
+        <v>58</v>
+      </c>
+      <c r="AB27" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC27" t="s">
+        <v>56</v>
+      </c>
+      <c r="AD27" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE27" t="s">
+        <v>58</v>
+      </c>
+      <c r="AF27" t="s">
+        <v>54</v>
+      </c>
+      <c r="AG27" t="s">
+        <v>58</v>
+      </c>
+      <c r="AH27" t="s">
+        <v>54</v>
+      </c>
+      <c r="AI27" t="s">
+        <v>54</v>
+      </c>
+      <c r="AJ27" t="s">
+        <v>54</v>
+      </c>
+      <c r="AK27" t="s">
+        <v>59</v>
+      </c>
+      <c r="AL27" t="s">
+        <v>54</v>
+      </c>
+      <c r="AM27" t="s">
+        <v>54</v>
+      </c>
+      <c r="AN27" t="s">
+        <v>54</v>
+      </c>
+      <c r="AO27" t="s">
+        <v>54</v>
+      </c>
+      <c r="AP27" t="s">
+        <v>58</v>
+      </c>
+      <c r="AQ27" t="s">
+        <v>54</v>
+      </c>
+      <c r="AR27" t="s">
+        <v>161</v>
+      </c>
+      <c r="AS27" t="s">
+        <v>54</v>
+      </c>
+      <c r="AT27" t="s">
+        <v>56</v>
+      </c>
+      <c r="AU27" t="s">
+        <v>56</v>
+      </c>
+      <c r="AV27" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="AW27" t="s">
+        <v>162</v>
+      </c>
+      <c r="AX27" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="28" spans="1:51" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>30</v>
+      </c>
+      <c r="B28" s="1">
+        <v>45608.581712963001</v>
+      </c>
+      <c r="C28" s="1">
+        <v>45608.585277777798</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="E28" t="s">
+        <v>52</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="G28" t="s">
+        <v>56</v>
+      </c>
+      <c r="H28" t="s">
+        <v>54</v>
+      </c>
+      <c r="I28" t="s">
+        <v>56</v>
+      </c>
+      <c r="J28" t="s">
+        <v>56</v>
+      </c>
+      <c r="K28" t="s">
+        <v>60</v>
+      </c>
+      <c r="L28" t="s">
+        <v>60</v>
+      </c>
+      <c r="M28" t="s">
+        <v>60</v>
+      </c>
+      <c r="N28" t="s">
+        <v>60</v>
+      </c>
+      <c r="O28" t="s">
+        <v>55</v>
+      </c>
+      <c r="P28" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q28" t="s">
+        <v>54</v>
+      </c>
+      <c r="R28" t="s">
+        <v>55</v>
+      </c>
+      <c r="S28" t="s">
+        <v>55</v>
+      </c>
+      <c r="T28" t="s">
+        <v>55</v>
+      </c>
+      <c r="U28" t="s">
+        <v>60</v>
+      </c>
+      <c r="V28" t="s">
+        <v>55</v>
+      </c>
+      <c r="W28" t="s">
+        <v>60</v>
+      </c>
+      <c r="X28" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y28" t="s">
+        <v>58</v>
+      </c>
+      <c r="Z28" t="s">
+        <v>54</v>
+      </c>
+      <c r="AA28" t="s">
+        <v>58</v>
+      </c>
+      <c r="AB28" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC28" t="s">
+        <v>58</v>
+      </c>
+      <c r="AD28" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE28" t="s">
+        <v>79</v>
+      </c>
+      <c r="AF28" t="s">
+        <v>54</v>
+      </c>
+      <c r="AG28" t="s">
+        <v>58</v>
+      </c>
+      <c r="AH28" t="s">
+        <v>56</v>
+      </c>
+      <c r="AI28" t="s">
+        <v>54</v>
+      </c>
+      <c r="AJ28" t="s">
+        <v>54</v>
+      </c>
+      <c r="AK28" t="s">
+        <v>120</v>
+      </c>
+      <c r="AL28" t="s">
+        <v>60</v>
+      </c>
+      <c r="AM28" t="s">
+        <v>60</v>
+      </c>
+      <c r="AN28" t="s">
+        <v>60</v>
+      </c>
+      <c r="AO28" t="s">
+        <v>60</v>
+      </c>
+      <c r="AP28" t="s">
+        <v>60</v>
+      </c>
+      <c r="AQ28" t="s">
+        <v>60</v>
+      </c>
+      <c r="AS28" t="s">
+        <v>58</v>
+      </c>
+      <c r="AT28" t="s">
+        <v>56</v>
+      </c>
+      <c r="AU28" t="s">
+        <v>56</v>
+      </c>
+      <c r="AV28" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="AW28" t="s">
+        <v>166</v>
+      </c>
+      <c r="AX28" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="29" spans="1:51" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>31</v>
+      </c>
+      <c r="B29" s="1">
+        <v>45608.582997685196</v>
+      </c>
+      <c r="C29" s="1">
+        <v>45608.586678240703</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="E29" t="s">
+        <v>52</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="G29" t="s">
+        <v>58</v>
+      </c>
+      <c r="H29" t="s">
+        <v>58</v>
+      </c>
+      <c r="I29" t="s">
+        <v>58</v>
+      </c>
+      <c r="J29" t="s">
+        <v>58</v>
+      </c>
+      <c r="K29" t="s">
+        <v>55</v>
+      </c>
+      <c r="L29" t="s">
+        <v>55</v>
+      </c>
+      <c r="M29" t="s">
+        <v>55</v>
+      </c>
+      <c r="N29" t="s">
+        <v>55</v>
+      </c>
+      <c r="O29" t="s">
+        <v>55</v>
+      </c>
+      <c r="P29" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q29" t="s">
+        <v>55</v>
+      </c>
+      <c r="R29" t="s">
+        <v>58</v>
+      </c>
+      <c r="S29" t="s">
+        <v>58</v>
+      </c>
+      <c r="T29" t="s">
+        <v>58</v>
+      </c>
+      <c r="U29" t="s">
+        <v>57</v>
+      </c>
+      <c r="V29" t="s">
+        <v>57</v>
+      </c>
+      <c r="W29" t="s">
+        <v>57</v>
+      </c>
+      <c r="X29" t="s">
+        <v>58</v>
+      </c>
+      <c r="Y29" t="s">
+        <v>58</v>
+      </c>
+      <c r="Z29" t="s">
+        <v>54</v>
+      </c>
+      <c r="AA29" t="s">
+        <v>58</v>
+      </c>
+      <c r="AB29" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC29" t="s">
+        <v>58</v>
+      </c>
+      <c r="AD29" t="s">
+        <v>56</v>
+      </c>
+      <c r="AE29" t="s">
+        <v>56</v>
+      </c>
+      <c r="AF29" t="s">
+        <v>56</v>
+      </c>
+      <c r="AG29" t="s">
+        <v>56</v>
+      </c>
+      <c r="AH29" t="s">
+        <v>54</v>
+      </c>
+      <c r="AI29" t="s">
+        <v>58</v>
+      </c>
+      <c r="AJ29" t="s">
+        <v>56</v>
+      </c>
+      <c r="AK29" t="s">
+        <v>74</v>
+      </c>
+      <c r="AL29" t="s">
+        <v>60</v>
+      </c>
+      <c r="AM29" t="s">
+        <v>58</v>
+      </c>
+      <c r="AN29" t="s">
+        <v>60</v>
+      </c>
+      <c r="AO29" t="s">
+        <v>60</v>
+      </c>
+      <c r="AP29" t="s">
+        <v>58</v>
+      </c>
+      <c r="AQ29" t="s">
+        <v>54</v>
+      </c>
+      <c r="AR29" t="s">
+        <v>168</v>
+      </c>
+      <c r="AS29" t="s">
+        <v>58</v>
+      </c>
+      <c r="AT29" t="s">
+        <v>58</v>
+      </c>
+      <c r="AU29" t="s">
+        <v>58</v>
+      </c>
+      <c r="AV29" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="AW29" t="s">
+        <v>169</v>
+      </c>
+      <c r="AX29" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="30" spans="1:51" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>32</v>
+      </c>
+      <c r="B30" s="1">
+        <v>45608.583425925899</v>
+      </c>
+      <c r="C30" s="1">
+        <v>45608.588449074101</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E30" t="s">
         <v>107</v>
       </c>
-      <c r="AW13" t="s">
-        <v>108</v>
+      <c r="F30" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="G30" t="s">
+        <v>56</v>
+      </c>
+      <c r="H30" t="s">
+        <v>54</v>
+      </c>
+      <c r="I30" t="s">
+        <v>55</v>
+      </c>
+      <c r="J30" t="s">
+        <v>56</v>
+      </c>
+      <c r="K30" t="s">
+        <v>54</v>
+      </c>
+      <c r="L30" t="s">
+        <v>54</v>
+      </c>
+      <c r="M30" t="s">
+        <v>54</v>
+      </c>
+      <c r="N30" t="s">
+        <v>56</v>
+      </c>
+      <c r="O30" t="s">
+        <v>54</v>
+      </c>
+      <c r="P30" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q30" t="s">
+        <v>56</v>
+      </c>
+      <c r="R30" t="s">
+        <v>60</v>
+      </c>
+      <c r="S30" t="s">
+        <v>54</v>
+      </c>
+      <c r="T30" t="s">
+        <v>54</v>
+      </c>
+      <c r="U30" t="s">
+        <v>60</v>
+      </c>
+      <c r="V30" t="s">
+        <v>54</v>
+      </c>
+      <c r="W30" t="s">
+        <v>54</v>
+      </c>
+      <c r="X30" t="s">
+        <v>54</v>
+      </c>
+      <c r="Y30" t="s">
+        <v>79</v>
+      </c>
+      <c r="Z30" t="s">
+        <v>54</v>
+      </c>
+      <c r="AA30" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB30" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC30" t="s">
+        <v>56</v>
+      </c>
+      <c r="AD30" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE30" t="s">
+        <v>79</v>
+      </c>
+      <c r="AF30" t="s">
+        <v>54</v>
+      </c>
+      <c r="AG30" t="s">
+        <v>79</v>
+      </c>
+      <c r="AH30" t="s">
+        <v>54</v>
+      </c>
+      <c r="AI30" t="s">
+        <v>54</v>
+      </c>
+      <c r="AJ30" t="s">
+        <v>54</v>
+      </c>
+      <c r="AK30" t="s">
+        <v>120</v>
+      </c>
+      <c r="AL30" t="s">
+        <v>60</v>
+      </c>
+      <c r="AM30" t="s">
+        <v>60</v>
+      </c>
+      <c r="AN30" t="s">
+        <v>60</v>
+      </c>
+      <c r="AO30" t="s">
+        <v>60</v>
+      </c>
+      <c r="AP30" t="s">
+        <v>60</v>
+      </c>
+      <c r="AQ30" t="s">
+        <v>54</v>
+      </c>
+      <c r="AS30" t="s">
+        <v>54</v>
+      </c>
+      <c r="AT30" t="s">
+        <v>56</v>
+      </c>
+      <c r="AU30" t="s">
+        <v>56</v>
+      </c>
+      <c r="AV30" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="AW30" t="s">
+        <v>171</v>
+      </c>
+      <c r="AY30" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="31" spans="1:51" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>33</v>
+      </c>
+      <c r="B31" s="1">
+        <v>45608.581921296303</v>
+      </c>
+      <c r="C31" s="1">
+        <v>45608.588738425897</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="E31" t="s">
+        <v>52</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="G31" t="s">
+        <v>54</v>
+      </c>
+      <c r="H31" t="s">
+        <v>56</v>
+      </c>
+      <c r="I31" t="s">
+        <v>56</v>
+      </c>
+      <c r="J31" t="s">
+        <v>56</v>
+      </c>
+      <c r="K31" t="s">
+        <v>55</v>
+      </c>
+      <c r="L31" t="s">
+        <v>55</v>
+      </c>
+      <c r="M31" t="s">
+        <v>55</v>
+      </c>
+      <c r="N31" t="s">
+        <v>56</v>
+      </c>
+      <c r="O31" t="s">
+        <v>56</v>
+      </c>
+      <c r="P31" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q31" t="s">
+        <v>55</v>
+      </c>
+      <c r="R31" t="s">
+        <v>56</v>
+      </c>
+      <c r="S31" t="s">
+        <v>56</v>
+      </c>
+      <c r="T31" t="s">
+        <v>56</v>
+      </c>
+      <c r="U31" t="s">
+        <v>55</v>
+      </c>
+      <c r="V31" t="s">
+        <v>55</v>
+      </c>
+      <c r="W31" t="s">
+        <v>55</v>
+      </c>
+      <c r="X31" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y31" t="s">
+        <v>58</v>
+      </c>
+      <c r="Z31" t="s">
+        <v>54</v>
+      </c>
+      <c r="AA31" t="s">
+        <v>56</v>
+      </c>
+      <c r="AB31" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC31" t="s">
+        <v>54</v>
+      </c>
+      <c r="AD31" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE31" t="s">
+        <v>58</v>
+      </c>
+      <c r="AF31" t="s">
+        <v>56</v>
+      </c>
+      <c r="AG31" t="s">
+        <v>58</v>
+      </c>
+      <c r="AH31" t="s">
+        <v>54</v>
+      </c>
+      <c r="AI31" t="s">
+        <v>58</v>
+      </c>
+      <c r="AJ31" t="s">
+        <v>56</v>
+      </c>
+      <c r="AK31" t="s">
+        <v>59</v>
+      </c>
+      <c r="AL31" t="s">
+        <v>54</v>
+      </c>
+      <c r="AM31" t="s">
+        <v>54</v>
+      </c>
+      <c r="AN31" t="s">
+        <v>54</v>
+      </c>
+      <c r="AO31" t="s">
+        <v>58</v>
+      </c>
+      <c r="AP31" t="s">
+        <v>54</v>
+      </c>
+      <c r="AQ31" t="s">
+        <v>54</v>
+      </c>
+      <c r="AS31" t="s">
+        <v>56</v>
+      </c>
+      <c r="AT31" t="s">
+        <v>58</v>
+      </c>
+      <c r="AU31" t="s">
+        <v>56</v>
+      </c>
+      <c r="AV31" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="AY31" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="32" spans="1:51" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>34</v>
+      </c>
+      <c r="B32" s="1">
+        <v>45608.582581018498</v>
+      </c>
+      <c r="C32" s="1">
+        <v>45608.592152777797</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="E32" t="s">
+        <v>52</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="G32" t="s">
+        <v>54</v>
+      </c>
+      <c r="H32" t="s">
+        <v>55</v>
+      </c>
+      <c r="I32" t="s">
+        <v>58</v>
+      </c>
+      <c r="J32" t="s">
+        <v>58</v>
+      </c>
+      <c r="K32" t="s">
+        <v>55</v>
+      </c>
+      <c r="L32" t="s">
+        <v>55</v>
+      </c>
+      <c r="M32" t="s">
+        <v>55</v>
+      </c>
+      <c r="N32" t="s">
+        <v>57</v>
+      </c>
+      <c r="O32" t="s">
+        <v>55</v>
+      </c>
+      <c r="P32" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q32" t="s">
+        <v>57</v>
+      </c>
+      <c r="R32" t="s">
+        <v>56</v>
+      </c>
+      <c r="S32" t="s">
+        <v>56</v>
+      </c>
+      <c r="T32" t="s">
+        <v>56</v>
+      </c>
+      <c r="U32" t="s">
+        <v>55</v>
+      </c>
+      <c r="V32" t="s">
+        <v>56</v>
+      </c>
+      <c r="W32" t="s">
+        <v>55</v>
+      </c>
+      <c r="X32" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y32" t="s">
+        <v>54</v>
+      </c>
+      <c r="Z32" t="s">
+        <v>58</v>
+      </c>
+      <c r="AA32" t="s">
+        <v>58</v>
+      </c>
+      <c r="AD32" t="s">
+        <v>58</v>
+      </c>
+      <c r="AE32" t="s">
+        <v>54</v>
+      </c>
+      <c r="AF32" t="s">
+        <v>54</v>
+      </c>
+      <c r="AG32" t="s">
+        <v>56</v>
+      </c>
+      <c r="AH32" t="s">
+        <v>54</v>
+      </c>
+      <c r="AI32" t="s">
+        <v>54</v>
+      </c>
+      <c r="AJ32" t="s">
+        <v>54</v>
+      </c>
+      <c r="AK32" t="s">
+        <v>59</v>
+      </c>
+      <c r="AL32" t="s">
+        <v>60</v>
+      </c>
+      <c r="AM32" t="s">
+        <v>54</v>
+      </c>
+      <c r="AN32" t="s">
+        <v>60</v>
+      </c>
+      <c r="AO32" t="s">
+        <v>54</v>
+      </c>
+      <c r="AP32" t="s">
+        <v>54</v>
+      </c>
+      <c r="AQ32" t="s">
+        <v>60</v>
+      </c>
+      <c r="AR32" t="s">
+        <v>174</v>
+      </c>
+      <c r="AS32" t="s">
+        <v>54</v>
+      </c>
+      <c r="AT32" t="s">
+        <v>58</v>
+      </c>
+      <c r="AU32" t="s">
+        <v>56</v>
+      </c>
+      <c r="AV32" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="AW32" t="s">
+        <v>176</v>
+      </c>
+      <c r="AX32" t="s">
+        <v>177</v>
+      </c>
+      <c r="AY32" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="33" spans="1:51" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>35</v>
+      </c>
+      <c r="B33" s="1">
+        <v>45608.587800925903</v>
+      </c>
+      <c r="C33" s="1">
+        <v>45608.599513888897</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="E33" t="s">
+        <v>52</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="G33" t="s">
+        <v>54</v>
+      </c>
+      <c r="H33" t="s">
+        <v>54</v>
+      </c>
+      <c r="I33" t="s">
+        <v>57</v>
+      </c>
+      <c r="J33" t="s">
+        <v>56</v>
+      </c>
+      <c r="K33" t="s">
+        <v>54</v>
+      </c>
+      <c r="L33" t="s">
+        <v>55</v>
+      </c>
+      <c r="M33" t="s">
+        <v>56</v>
+      </c>
+      <c r="N33" t="s">
+        <v>56</v>
+      </c>
+      <c r="O33" t="s">
+        <v>54</v>
+      </c>
+      <c r="P33" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q33" t="s">
+        <v>55</v>
+      </c>
+      <c r="R33" t="s">
+        <v>55</v>
+      </c>
+      <c r="S33" t="s">
+        <v>55</v>
+      </c>
+      <c r="T33" t="s">
+        <v>55</v>
+      </c>
+      <c r="U33" t="s">
+        <v>54</v>
+      </c>
+      <c r="V33" t="s">
+        <v>55</v>
+      </c>
+      <c r="W33" t="s">
+        <v>60</v>
+      </c>
+      <c r="X33" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y33" t="s">
+        <v>58</v>
+      </c>
+      <c r="Z33" t="s">
+        <v>54</v>
+      </c>
+      <c r="AA33" t="s">
+        <v>56</v>
+      </c>
+      <c r="AB33" t="s">
+        <v>56</v>
+      </c>
+      <c r="AC33" t="s">
+        <v>56</v>
+      </c>
+      <c r="AD33" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE33" t="s">
+        <v>56</v>
+      </c>
+      <c r="AF33" t="s">
+        <v>58</v>
+      </c>
+      <c r="AG33" t="s">
+        <v>56</v>
+      </c>
+      <c r="AH33" t="s">
+        <v>54</v>
+      </c>
+      <c r="AI33" t="s">
+        <v>54</v>
+      </c>
+      <c r="AJ33" t="s">
+        <v>56</v>
+      </c>
+      <c r="AK33" t="s">
+        <v>59</v>
+      </c>
+      <c r="AL33" t="s">
+        <v>60</v>
+      </c>
+      <c r="AM33" t="s">
+        <v>60</v>
+      </c>
+      <c r="AN33" t="s">
+        <v>60</v>
+      </c>
+      <c r="AO33" t="s">
+        <v>60</v>
+      </c>
+      <c r="AP33" t="s">
+        <v>60</v>
+      </c>
+      <c r="AQ33" t="s">
+        <v>60</v>
+      </c>
+      <c r="AR33" t="s">
+        <v>179</v>
+      </c>
+      <c r="AS33" t="s">
+        <v>54</v>
+      </c>
+      <c r="AT33" t="s">
+        <v>56</v>
+      </c>
+      <c r="AU33" t="s">
+        <v>56</v>
+      </c>
+      <c r="AV33" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="AW33" t="s">
+        <v>180</v>
+      </c>
+      <c r="AX33" t="s">
+        <v>181</v>
+      </c>
+      <c r="AY33" t="s">
+        <v>182</v>
       </c>
     </row>
   </sheetData>

</xml_diff>